<commit_message>
Update 10 Content Pack D365Basics.xlsx
</commit_message>
<xml_diff>
--- a/10 Content Pack D365Basics.xlsx
+++ b/10 Content Pack D365Basics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-mluubach\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maik\Documents\GitHub\calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A6127A-181F-4EF4-8BA2-0CC9B234B937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7CC786-83E9-43BC-8B05-F7BF7FE392A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33885" yWindow="-18150" windowWidth="7050" windowHeight="3840" xr2:uid="{36ACBFC6-48A0-4CD7-B10E-9675CF43A6CD}"/>
+    <workbookView xWindow="5280" yWindow="3984" windowWidth="34560" windowHeight="13644" xr2:uid="{36ACBFC6-48A0-4CD7-B10E-9675CF43A6CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -71,9 +70,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Power Platform</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=-cq6s_0BWjc</t>
   </si>
   <si>
@@ -123,6 +119,9 @@
   </si>
   <si>
     <t>https://lifelikemaik.github.io/calendar/d365traincertdeck.png</t>
+  </si>
+  <si>
+    <t>D365</t>
   </si>
 </sst>
 </file>
@@ -527,20 +526,20 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="114.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="114.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,9 +559,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1">
         <v>44531</v>
@@ -571,15 +570,15 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
         <v>44532</v>
@@ -588,18 +587,18 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>44533</v>
@@ -608,18 +607,18 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <v>44534</v>
@@ -628,18 +627,18 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
         <v>44535</v>
@@ -648,18 +647,18 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
         <v>44536</v>
@@ -668,18 +667,18 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1">
         <v>44537</v>
@@ -688,18 +687,18 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>44538</v>
@@ -708,18 +707,18 @@
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1">
         <v>44539</v>
@@ -728,18 +727,18 @@
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1">
         <v>44540</v>
@@ -801,32 +800,32 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.265625" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -840,92 +839,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Owner xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Math_Settings xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <TeamsChannelId xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <NotebookType xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Students xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Has_Leaders_Only_SectionGroup xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AppVersion xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <CultureName xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Distribution_Groups xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Templates xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Members xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Invited_Teachers xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Invited_Students xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <FolderType xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Teachers xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Leaders xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <Member_Groups xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <Invited_Members xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <LMS_Mappings xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-    <Invited_Leaders xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100777DB4BD9E953546B515946AF28F7DA9" ma:contentTypeVersion="42" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c0da4c0e7967ab90613fc23f763a5156">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="7011d684-d841-471c-9031-84b0b301070d" xmlns:ns4="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="931b6df896159ff5736adb0b1c9a3ae0" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1441,26 +1354,93 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0A4B2C-23E9-4600-B233-DC08F6478FEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEB5A595-6ECE-49F1-AADE-0218D6C158AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Owner xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Math_Settings xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <TeamsChannelId xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <NotebookType xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Students xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Has_Leaders_Only_SectionGroup xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <AppVersion xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <CultureName xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Distribution_Groups xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Templates xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Members xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Invited_Teachers xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Invited_Students xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <FolderType xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Teachers xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Leaders xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <Member_Groups xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <Invited_Members xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <LMS_Mappings xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+    <Invited_Leaders xmlns="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A57166B1-F307-4C58-BB14-04F71658D735}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1480,6 +1460,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEB5A595-6ECE-49F1-AADE-0218D6C158AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0A4B2C-23E9-4600-B233-DC08F6478FEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bb4ef2a3-abf9-4bd1-87ad-3597e77c0e6c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>